<commit_message>
Fixed release column by changing it to year only
</commit_message>
<xml_diff>
--- a/converting_excel_to_psml/Movie_extra.xlsx
+++ b/converting_excel_to_psml/Movie_extra.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\atemp\liz\Movies\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-15" yWindow="5775" windowWidth="23250" windowHeight="5835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
   <si>
     <t>Annie Hall</t>
   </si>
@@ -95,9 +90,6 @@
  </t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Big Night</t>
   </si>
   <si>
@@ -251,19 +243,16 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>an_ID</t>
-  </si>
-  <si>
-    <t>dd/mm/yyyy</t>
-  </si>
-  <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>yyyy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -332,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -349,26 +338,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -395,6 +372,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,14 +409,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>47626</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
@@ -434,7 +426,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B2A66A3-4869-49B9-B181-8BFA8A307521}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2B2A66A3-4869-49B9-B181-8BFA8A307521}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -442,8 +434,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11144250" y="1028701"/>
-          <a:ext cx="4619626" cy="1657350"/>
+          <a:off x="9296400" y="1028701"/>
+          <a:ext cx="4648200" cy="1657350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -799,7 +791,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -807,624 +799,571 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="26.125" customWidth="1"/>
-    <col min="8" max="8" width="41.125" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="19" t="s">
+      <c r="B2" s="20">
+        <v>1977</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6">
-        <v>31100</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="B3" s="20">
+        <v>1985</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6">
-        <v>15097</v>
-      </c>
-      <c r="D4" s="19" t="s">
+      <c r="B4" s="20">
+        <v>1941</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="20">
+        <v>1996</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1">
-        <v>135855</v>
-      </c>
-      <c r="C5" s="6">
-        <v>35088</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="20">
+        <v>1983</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1">
-        <v>72689</v>
-      </c>
-      <c r="C6" s="6">
-        <v>30568</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="20">
+        <v>1980</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5460</v>
-      </c>
-      <c r="C7" s="6">
-        <v>29357</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="G7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="H7" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="20">
+        <v>1970</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="1">
-        <v>29499</v>
-      </c>
-      <c r="C8" s="6">
-        <v>25916</v>
-      </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="20">
+        <v>1958</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="20">
+        <v>1953</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="G10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="20">
+        <v>1952</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="20">
+        <v>1948</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="20">
+        <v>1947</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="20">
+        <v>1946</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="13" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="1">
-        <v>5408</v>
-      </c>
-      <c r="C9" s="6">
-        <v>21385</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="1">
-        <v>5428</v>
-      </c>
-      <c r="C10" s="6">
-        <v>19646</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="1">
-        <v>5470</v>
-      </c>
-      <c r="C11" s="6">
-        <v>19204</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="1">
-        <v>84976</v>
-      </c>
-      <c r="C12" s="6">
-        <v>17611</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="1">
-        <v>32831</v>
-      </c>
-      <c r="C13" s="6">
-        <v>17322</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="1">
-        <v>5471</v>
-      </c>
-      <c r="C14" s="6">
-        <v>17036</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="17" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="20" t="s">
+      <c r="E15" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>